<commit_message>
additions and correctios to the code, added asertion after adding new contact
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BHAKTI\Selenium Automation Projects\FreeCRMTest\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AA53F0-D7D9-44FD-A7D4-2BB94F8EF42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB547CBD-6434-4459-9E2D-D0E6855904FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CDDED0DE-552D-4928-BDBD-229BE5525C08}"/>
+    <workbookView xWindow="348" yWindow="348" windowWidth="19500" windowHeight="9972" xr2:uid="{CDDED0DE-552D-4928-BDBD-229BE5525C08}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -449,7 +440,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>